<commit_message>
add motion blur acceleration structure as additional feature
</commit_message>
<xml_diff>
--- a/final-project-workload-final.xlsx
+++ b/final-project-workload-final.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thijs\TU Delft\CG\final\template-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89182612-2C77-4951-8B4E-8800EAAF0B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7176" tabRatio="500"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workload" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <definedName name="_56F9DC9755BA473782653E2940F9ResponseSheet">"Form1"</definedName>
     <definedName name="_56F9DC9755BA473782653E2940F9SourceDocId">"{1ec53893-4bf9-4845-bb1e-7f11035496d8}"</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>FILL IN THE BLUE BOXES ONLY</t>
   </si>
@@ -131,13 +132,19 @@
   </si>
   <si>
     <t>Paul Anton</t>
+  </si>
+  <si>
+    <t>Addition features</t>
+  </si>
+  <si>
+    <t>Motion blur acceleration structure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +197,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -308,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -398,6 +412,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -781,11 +798,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,6 +1273,28 @@
         <v>10.5</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="27"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
+        <v>100</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
@@ -1267,7 +1306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>